<commit_message>
Actualización automática de datos
</commit_message>
<xml_diff>
--- a/stilos_kids.xlsx
+++ b/stilos_kids.xlsx
@@ -614,11 +614,11 @@
         </is>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>vidal</t>
+          <t>mario</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">

</xml_diff>